<commit_message>
typo fix in candidates 2016
</commit_message>
<xml_diff>
--- a/US/example/primary_iowa_2016/candidates_2016.xlsx
+++ b/US/example/primary_iowa_2016/candidates_2016.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10400" yWindow="0" windowWidth="25360" windowHeight="14100" tabRatio="500"/>
+    <workbookView xWindow="1240" yWindow="0" windowWidth="25360" windowHeight="13940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="133">
   <si>
     <t>id</t>
   </si>
@@ -415,6 +415,9 @@
   </si>
   <si>
     <t>#b15928</t>
+  </si>
+  <si>
+    <t>#cccccc</t>
   </si>
 </sst>
 </file>
@@ -857,7 +860,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1422,7 +1425,7 @@
         <v>26</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1445,7 +1448,7 @@
         <v>26</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1468,7 +1471,7 @@
         <v>26</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1491,7 +1494,7 @@
         <v>26</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1514,7 +1517,7 @@
         <v>26</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1537,7 +1540,7 @@
         <v>39</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="3" customFormat="1">
@@ -1583,7 +1586,7 @@
         <v>92</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>